<commit_message>
fixes for empty cells and sessions processing
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/agegroups/USAW-AgeGroups_en.xlsx
+++ b/owlcms/src/main/resources/agegroups/USAW-AgeGroups_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\agegroups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F9103D-2917-4686-97A6-19E838F803C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86F9A79-C32B-4C1E-BEC8-49CFBBF8DE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="1335" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3255" yWindow="900" windowWidth="21600" windowHeight="12645" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AgeGroups" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="75">
   <si>
     <t>code</t>
   </si>
@@ -233,6 +232,33 @@
   </si>
   <si>
     <t>M80</t>
+  </si>
+  <si>
+    <t>W80</t>
+  </si>
+  <si>
+    <t>W85</t>
+  </si>
+  <si>
+    <t>W90</t>
+  </si>
+  <si>
+    <t>W95</t>
+  </si>
+  <si>
+    <t>W100</t>
+  </si>
+  <si>
+    <t>M85</t>
+  </si>
+  <si>
+    <t>M90</t>
+  </si>
+  <si>
+    <t>M95</t>
+  </si>
+  <si>
+    <t>M100</t>
   </si>
 </sst>
 </file>
@@ -693,9 +719,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W1048576"/>
+  <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40:G41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1374,7 +1402,7 @@
         <v>75</v>
       </c>
       <c r="F13" s="3">
-        <v>999</v>
+        <v>79</v>
       </c>
       <c r="G13" s="5" t="b">
         <f>FALSE()</f>
@@ -1417,24 +1445,24 @@
     </row>
     <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="3">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="F14" s="3">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="G14" s="5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H14" s="1"/>
       <c r="K14" s="1"/>
@@ -1473,20 +1501,20 @@
     </row>
     <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="3">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="F15" s="3">
-        <v>999</v>
+        <v>89</v>
       </c>
       <c r="G15" s="5" t="b">
         <f>FALSE()</f>
@@ -1527,31 +1555,29 @@
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="3">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F16" s="3">
-        <v>999</v>
+        <v>94</v>
       </c>
       <c r="G16" s="5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="K16" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1585,134 +1611,134 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E17" s="3">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="F17" s="3">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="G17" s="5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I17" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" t="s">
-        <v>57</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>58</v>
-      </c>
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="K17" s="1"/>
       <c r="L17" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="V17" s="1"/>
-    </row>
-    <row r="18" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="W17" s="1"/>
+    </row>
+    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E18" s="3">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="F18" s="3">
-        <v>15</v>
+        <v>999</v>
       </c>
       <c r="G18" s="5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="J18" t="s">
-        <v>57</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="K18" s="1"/>
       <c r="L18" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U18" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="V18" s="1"/>
-    </row>
-    <row r="19" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="W18" s="1"/>
+    </row>
+    <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E19" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F19" s="3">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G19" s="5" t="b">
         <f>TRUE()</f>
@@ -1721,171 +1747,188 @@
       <c r="H19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="V19" s="1"/>
-    </row>
-    <row r="20" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="W19" s="1"/>
+    </row>
+    <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="F20" s="3">
-        <v>39</v>
+        <v>999</v>
       </c>
       <c r="G20" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="M20" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+    </row>
+    <row r="21" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E21" s="3">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F21" s="3">
-        <v>44</v>
+        <v>999</v>
       </c>
       <c r="G21" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="M21" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+    </row>
+    <row r="22" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="F22" s="3">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="G22" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" t="s">
+        <v>57</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1899,48 +1942,45 @@
         <v>9</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V22" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+    </row>
+    <row r="23" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="3">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="F23" s="3">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="G23" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="J23" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M23" s="1" t="s">
         <v>6</v>
       </c>
@@ -1960,42 +2000,37 @@
         <v>11</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V23" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+    </row>
+    <row r="24" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="3">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="F24" s="3">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="G24" s="5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
+      <c r="L24" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="M24" s="1" t="s">
         <v>6</v>
       </c>
@@ -2021,15 +2056,13 @@
         <v>13</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V24" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="V24" s="1"/>
+    </row>
+    <row r="25" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
@@ -2039,10 +2072,10 @@
         <v>3</v>
       </c>
       <c r="E25" s="3">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="F25" s="3">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="G25" s="5" t="b">
         <f>FALSE()</f>
@@ -2082,9 +2115,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
@@ -2094,10 +2127,10 @@
         <v>3</v>
       </c>
       <c r="E26" s="3">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="F26" s="3">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="G26" s="5" t="b">
         <f>FALSE()</f>
@@ -2137,9 +2170,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>4</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
@@ -2149,10 +2182,10 @@
         <v>3</v>
       </c>
       <c r="E27" s="3">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="F27" s="3">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="G27" s="5" t="b">
         <f>FALSE()</f>
@@ -2192,9 +2225,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
@@ -2204,10 +2237,10 @@
         <v>3</v>
       </c>
       <c r="E28" s="3">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F28" s="3">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="G28" s="5" t="b">
         <f>FALSE()</f>
@@ -2247,9 +2280,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>65</v>
+    <row r="29" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
@@ -2259,10 +2292,10 @@
         <v>3</v>
       </c>
       <c r="E29" s="3">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="F29" s="3">
-        <v>999</v>
+        <v>59</v>
       </c>
       <c r="G29" s="5" t="b">
         <f>FALSE()</f>
@@ -2302,26 +2335,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="3">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F30" s="3">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="G30" s="5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H30" s="1"/>
       <c r="K30" s="1"/>
@@ -2357,22 +2390,22 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="3">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="F31" s="3">
-        <v>999</v>
+        <v>69</v>
       </c>
       <c r="G31" s="5" t="b">
         <f>FALSE()</f>
@@ -2412,64 +2445,558 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="3">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F32" s="3">
+        <v>74</v>
+      </c>
+      <c r="G32" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="3">
+        <v>75</v>
+      </c>
+      <c r="F33" s="3">
+        <v>79</v>
+      </c>
+      <c r="G33" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V33" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="3">
+        <v>80</v>
+      </c>
+      <c r="F34" s="3">
+        <v>84</v>
+      </c>
+      <c r="G34" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="3">
+        <v>85</v>
+      </c>
+      <c r="F35" s="3">
+        <v>89</v>
+      </c>
+      <c r="G35" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V35" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="3">
+        <v>90</v>
+      </c>
+      <c r="F36" s="3">
+        <v>99</v>
+      </c>
+      <c r="G36" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>95</v>
+      </c>
+      <c r="F37" s="3">
+        <v>99</v>
+      </c>
+      <c r="G37" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="3">
+        <v>100</v>
+      </c>
+      <c r="F38" s="3">
         <v>999</v>
       </c>
-      <c r="G32" s="5" t="b">
+      <c r="G38" s="5" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V38" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="3">
+        <v>15</v>
+      </c>
+      <c r="F39" s="3">
+        <v>20</v>
+      </c>
+      <c r="G39" s="5" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1" t="s">
+      <c r="H39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V39" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3">
+        <v>15</v>
+      </c>
+      <c r="F40" s="3">
+        <v>999</v>
+      </c>
+      <c r="G40" s="5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V40" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3">
+        <v>999</v>
+      </c>
+      <c r="G41" s="5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="M41" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="N41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="O41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P32" s="1" t="s">
+      <c r="P41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="Q41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="R32" s="1" t="s">
+      <c r="R41" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S32" s="1" t="s">
+      <c r="S41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T32" s="1" t="s">
+      <c r="T41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="U32" s="1" t="s">
+      <c r="U41" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V32" s="1" t="s">
+      <c r="V41" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="1048576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
USAW Age Groups: Remove spurious weight classes
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/agegroups/USAW-AgeGroups_en.xlsx
+++ b/owlcms/src/main/resources/agegroups/USAW-AgeGroups_en.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottgonzalez/Projects/Misc/owlcms4/owlcms/src/main/resources/agegroups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFBE2DF-F16F-6E42-BED0-F57CFE3CEB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCFDA96-3FF8-6548-9E8C-4358094564EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1460" yWindow="500" windowWidth="26540" windowHeight="21420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="57">
   <si>
     <t>code</t>
   </si>
@@ -195,6 +195,18 @@
   </si>
   <si>
     <t>Adaptive</t>
+  </si>
+  <si>
+    <t>Youth</t>
+  </si>
+  <si>
+    <t>Juniors</t>
+  </si>
+  <si>
+    <t>Masters</t>
+  </si>
+  <si>
+    <t>Seniors</t>
   </si>
 </sst>
 </file>
@@ -588,7 +600,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -647,7 +659,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>9</v>
@@ -706,7 +718,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -764,7 +776,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
@@ -822,7 +834,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -880,7 +892,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
@@ -938,7 +950,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>17</v>
@@ -996,7 +1008,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
@@ -1054,7 +1066,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
@@ -1112,7 +1124,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -1170,7 +1182,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>17</v>
@@ -1228,7 +1240,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>17</v>
@@ -1286,7 +1298,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>17</v>
@@ -1344,7 +1356,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
@@ -1402,7 +1414,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -1460,7 +1472,7 @@
         <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>17</v>
@@ -1518,7 +1530,7 @@
         <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>17</v>
@@ -1576,7 +1588,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>17</v>
@@ -1634,7 +1646,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>17</v>
@@ -1692,7 +1704,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>17</v>
@@ -1750,7 +1762,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>32</v>
@@ -1808,7 +1820,7 @@
         <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -1885,9 +1897,7 @@
         <v>1</v>
       </c>
       <c r="H24" s="1"/>
-      <c r="K24" s="1">
-        <v>40</v>
-      </c>
+      <c r="K24" s="1"/>
       <c r="L24" s="1">
         <v>45</v>
       </c>
@@ -1945,9 +1955,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="K25" s="1">
-        <v>40</v>
-      </c>
+      <c r="K25" s="1"/>
       <c r="L25" s="1">
         <v>45</v>
       </c>
@@ -1986,7 +1994,7 @@
         <v>8</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>9</v>
@@ -2045,7 +2053,7 @@
         <v>11</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>9</v>
@@ -2104,7 +2112,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>9</v>
@@ -2161,7 +2169,7 @@
         <v>13</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>9</v>
@@ -2218,7 +2226,7 @@
         <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>9</v>
@@ -2275,7 +2283,7 @@
         <v>15</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>9</v>
@@ -2332,7 +2340,7 @@
         <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>17</v>
@@ -2389,7 +2397,7 @@
         <v>38</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>17</v>
@@ -2446,7 +2454,7 @@
         <v>39</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>17</v>
@@ -2503,7 +2511,7 @@
         <v>40</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>17</v>
@@ -2560,7 +2568,7 @@
         <v>41</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>17</v>
@@ -2617,7 +2625,7 @@
         <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>17</v>
@@ -2674,7 +2682,7 @@
         <v>43</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>17</v>
@@ -2731,7 +2739,7 @@
         <v>44</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>17</v>
@@ -2788,7 +2796,7 @@
         <v>45</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>17</v>
@@ -2845,7 +2853,7 @@
         <v>46</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>17</v>
@@ -2902,7 +2910,7 @@
         <v>47</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>17</v>
@@ -2959,7 +2967,7 @@
         <v>48</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>17</v>
@@ -3016,7 +3024,7 @@
         <v>49</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>17</v>
@@ -3073,7 +3081,7 @@
         <v>50</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>17</v>
@@ -3130,7 +3138,7 @@
         <v>31</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
@@ -3187,7 +3195,7 @@
         <v>33</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>32</v>

</xml_diff>